<commit_message>
Cleaning and adding data.
</commit_message>
<xml_diff>
--- a/src/bookofmagnus/books.xlsx
+++ b/src/bookofmagnus/books.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jennie\Documents\personal\repos\BookOfMagnus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jennie\Documents\personal\repos\BookOfMagnus\src\bookofmagnus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FC2378D-28FF-4CDC-BFFA-CD9360535917}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254284A4-1B73-45CF-A796-93CDBF12F21F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{081CEC6C-671A-4C6D-9320-71B970466DA2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{081CEC6C-671A-4C6D-9320-71B970466DA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="58">
   <si>
     <t>Title</t>
   </si>
@@ -199,13 +199,19 @@
   </si>
   <si>
     <t>Angels of Caliban</t>
+  </si>
+  <si>
+    <t>Follows</t>
+  </si>
+  <si>
+    <t>A Thousand Sons,Tales of Heresy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +232,19 @@
       <sz val="10"/>
       <color rgb="FF0B5394"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -248,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -259,6 +278,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,15 +597,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EFFEC2-FF66-493C-91A3-F32744CC455D}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C51"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,8 +619,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -602,8 +633,9 @@
       <c r="C2" s="4">
         <v>2006</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -613,8 +645,11 @@
       <c r="C3" s="4">
         <v>2006</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -624,8 +659,11 @@
       <c r="C4" s="4">
         <v>2006</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -635,8 +673,11 @@
       <c r="C5" s="4">
         <v>2007</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -646,8 +687,11 @@
       <c r="C6" s="4">
         <v>2007</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -657,8 +701,9 @@
       <c r="C7" s="4">
         <v>2007</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -668,8 +713,9 @@
       <c r="C8" s="4">
         <v>2008</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -679,8 +725,9 @@
       <c r="C9" s="4">
         <v>2008</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -690,9 +737,12 @@
       <c r="C10" s="4">
         <v>2008</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -701,8 +751,11 @@
       <c r="C11" s="4">
         <v>2009</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -712,8 +765,11 @@
       <c r="C12" s="4">
         <v>2009</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -723,8 +779,9 @@
       <c r="C13" s="4">
         <v>2009</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -734,8 +791,11 @@
       <c r="C14" s="4">
         <v>2010</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -745,8 +805,11 @@
       <c r="C15" s="4">
         <v>2010</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -756,8 +819,11 @@
       <c r="C16" s="4">
         <v>2010</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -767,8 +833,9 @@
       <c r="C17" s="4">
         <v>2011</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -778,8 +845,11 @@
       <c r="C18" s="4">
         <v>2011</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
@@ -789,8 +859,11 @@
       <c r="C19" s="4">
         <v>2011</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>23</v>
       </c>
@@ -800,8 +873,9 @@
       <c r="C20" s="4">
         <v>2011</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -811,8 +885,11 @@
       <c r="C21" s="4">
         <v>2011</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
@@ -822,8 +899,9 @@
       <c r="C22" s="4">
         <v>2012</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -833,8 +911,9 @@
       <c r="C23" s="4">
         <v>2012</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -844,8 +923,9 @@
       <c r="C24" s="4">
         <v>2012</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
@@ -855,8 +935,9 @@
       <c r="C25" s="4">
         <v>2012</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
@@ -866,8 +947,11 @@
       <c r="C26" s="4">
         <v>2012</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
@@ -877,8 +961,9 @@
       <c r="C27" s="4">
         <v>2012</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
@@ -888,8 +973,9 @@
       <c r="C28" s="4">
         <v>2013</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
@@ -899,8 +985,9 @@
       <c r="C29" s="4">
         <v>2013</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>34</v>
       </c>
@@ -910,8 +997,9 @@
       <c r="C30" s="4">
         <v>2013</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
@@ -921,8 +1009,9 @@
       <c r="C31" s="4">
         <v>2013</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>36</v>
       </c>
@@ -932,8 +1021,9 @@
       <c r="C32" s="4">
         <v>2013</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>37</v>
       </c>
@@ -943,8 +1033,9 @@
       <c r="C33" s="4">
         <v>2013</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>38</v>
       </c>
@@ -954,8 +1045,9 @@
       <c r="C34" s="4">
         <v>2014</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>39</v>
       </c>
@@ -965,8 +1057,9 @@
       <c r="C35" s="4">
         <v>2014</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>40</v>
       </c>
@@ -976,8 +1069,9 @@
       <c r="C36" s="4">
         <v>2014</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>41</v>
       </c>
@@ -987,8 +1081,9 @@
       <c r="C37" s="4">
         <v>2014</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>42</v>
       </c>
@@ -998,8 +1093,9 @@
       <c r="C38" s="4">
         <v>2014</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>43</v>
       </c>
@@ -1009,8 +1105,9 @@
       <c r="C39" s="4">
         <v>2014</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>44</v>
       </c>
@@ -1020,8 +1117,9 @@
       <c r="C40" s="4">
         <v>2015</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
@@ -1031,8 +1129,9 @@
       <c r="C41" s="4">
         <v>2015</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>46</v>
       </c>
@@ -1042,8 +1141,9 @@
       <c r="C42" s="4">
         <v>2015</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
@@ -1053,8 +1153,9 @@
       <c r="C43" s="4">
         <v>2015</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>48</v>
       </c>
@@ -1064,8 +1165,9 @@
       <c r="C44" s="4">
         <v>2015</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>49</v>
       </c>
@@ -1075,8 +1177,9 @@
       <c r="C45" s="4">
         <v>2015</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>50</v>
       </c>
@@ -1086,8 +1189,9 @@
       <c r="C46" s="4">
         <v>2016</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>51</v>
       </c>
@@ -1097,8 +1201,9 @@
       <c r="C47" s="4">
         <v>2016</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
@@ -1108,8 +1213,9 @@
       <c r="C48" s="4">
         <v>2016</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>53</v>
       </c>
@@ -1119,8 +1225,9 @@
       <c r="C49" s="4">
         <v>2016</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>54</v>
       </c>
@@ -1130,8 +1237,9 @@
       <c r="C50" s="4">
         <v>2016</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>55</v>
       </c>
@@ -1141,8 +1249,10 @@
       <c r="C51" s="4">
         <v>2016</v>
       </c>
+      <c r="D51" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>